<commit_message>
filled the normalizer and deleter with a multitude phrases and words to look for. Added more categories for the sorter to sort in the excel file
</commit_message>
<xml_diff>
--- a/1.Webscraper/Index.xlsx
+++ b/1.Webscraper/Index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikol\Noty-Database\1.Webscraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466EA568-E6BB-4075-BF3F-FDAD1C7FC673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCFCD0E-7B0D-4636-9231-5CFB37887671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="348">
   <si>
     <t>Categories/Occasions</t>
   </si>
@@ -273,9 +273,6 @@
     <t>Фортепиано</t>
   </si>
   <si>
-    <t>Фортепианный акк.</t>
-  </si>
-  <si>
     <t>Орган</t>
   </si>
   <si>
@@ -291,9 +288,6 @@
     <t>Album</t>
   </si>
   <si>
-    <t>Choir SATB</t>
-  </si>
-  <si>
     <t>Хор - Общее пение</t>
   </si>
   <si>
@@ -352,6 +346,744 @@
   </si>
   <si>
     <t>Тюрингская мелодия</t>
+  </si>
+  <si>
+    <t>Другой текст</t>
+  </si>
+  <si>
+    <t>Муж. 3-о</t>
+  </si>
+  <si>
+    <t>Оригинал</t>
+  </si>
+  <si>
+    <t>Українська народна колядка</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Українські слова</t>
+  </si>
+  <si>
+    <t>Хор - украинские варианты</t>
+  </si>
+  <si>
+    <t>Трубы 2-т</t>
+  </si>
+  <si>
+    <t>3-o - English</t>
+  </si>
+  <si>
+    <t>3-о - Русский</t>
+  </si>
+  <si>
+    <t>Хор - русский вариант</t>
+  </si>
+  <si>
+    <t>Виолончель</t>
+  </si>
+  <si>
+    <t>The Crossroads</t>
+  </si>
+  <si>
+    <t>Украинский вариант</t>
+  </si>
+  <si>
+    <t>Соло альт</t>
+  </si>
+  <si>
+    <t>Другая версия</t>
+  </si>
+  <si>
+    <t>На английском языке</t>
+  </si>
+  <si>
+    <t>В.Н. Степанов</t>
+  </si>
+  <si>
+    <t>Е. Бондарева</t>
+  </si>
+  <si>
+    <t>В. Стрелков</t>
+  </si>
+  <si>
+    <t>Д. Махмуд-Оглы</t>
+  </si>
+  <si>
+    <t>Чесноков</t>
+  </si>
+  <si>
+    <t>Сергей Воробьёв</t>
+  </si>
+  <si>
+    <t>Яворивский А.П.</t>
+  </si>
+  <si>
+    <t>Маген Станислав</t>
+  </si>
+  <si>
+    <t>John E. Walvoord</t>
+  </si>
+  <si>
+    <t>Don Wyrtzen</t>
+  </si>
+  <si>
+    <t>Л.В. Бетховен</t>
+  </si>
+  <si>
+    <t>Д. Простомолотов</t>
+  </si>
+  <si>
+    <t>Елена Дюкова</t>
+  </si>
+  <si>
+    <t>В.И. Павлов</t>
+  </si>
+  <si>
+    <t>Маршнер</t>
+  </si>
+  <si>
+    <t>С.А. Бацук</t>
+  </si>
+  <si>
+    <t>Гр. Кендрик</t>
+  </si>
+  <si>
+    <t>J. H. Tenney</t>
+  </si>
+  <si>
+    <t>Денис Пацюк</t>
+  </si>
+  <si>
+    <t>Ph.P. Bliss</t>
+  </si>
+  <si>
+    <t>Г. Конради</t>
+  </si>
+  <si>
+    <t>И.С. Проханов</t>
+  </si>
+  <si>
+    <t>В. Буду</t>
+  </si>
+  <si>
+    <t>Л Симонова</t>
+  </si>
+  <si>
+    <t>Я. Бузинский</t>
+  </si>
+  <si>
+    <t>Е. Гончаренко</t>
+  </si>
+  <si>
+    <t>М. Парафейник</t>
+  </si>
+  <si>
+    <t>В. Яцюк</t>
+  </si>
+  <si>
+    <t>Гапонюк Андрей</t>
+  </si>
+  <si>
+    <t>J. Macy</t>
+  </si>
+  <si>
+    <t>Dan and Heidi Goeller</t>
+  </si>
+  <si>
+    <t>Е Кашина</t>
+  </si>
+  <si>
+    <t>С Перебиковский</t>
+  </si>
+  <si>
+    <t>В. Перебиковский</t>
+  </si>
+  <si>
+    <t>С Шинкарёва</t>
+  </si>
+  <si>
+    <t>А Каргопольцев-В Петреченко</t>
+  </si>
+  <si>
+    <t>А. Гинтер</t>
+  </si>
+  <si>
+    <t>В. Мысин</t>
+  </si>
+  <si>
+    <t>Гурт Ковчег</t>
+  </si>
+  <si>
+    <t>Н. Николенко</t>
+  </si>
+  <si>
+    <t>Л. Клочкова</t>
+  </si>
+  <si>
+    <t>М. Кривошеев</t>
+  </si>
+  <si>
+    <t>Р. Голкина</t>
+  </si>
+  <si>
+    <t>Ю Аксенова</t>
+  </si>
+  <si>
+    <t>Н. Шалатовский</t>
+  </si>
+  <si>
+    <t>Я. Гильбург</t>
+  </si>
+  <si>
+    <t>F.E.Belden</t>
+  </si>
+  <si>
+    <t>Г Ф Львовский</t>
+  </si>
+  <si>
+    <t>Ремизов Е.П.</t>
+  </si>
+  <si>
+    <t>А. Денисова</t>
+  </si>
+  <si>
+    <t>А. Чипилка</t>
+  </si>
+  <si>
+    <t>Галина Александровна Везикова</t>
+  </si>
+  <si>
+    <t>Я. Крючковская</t>
+  </si>
+  <si>
+    <t>Е. Андрюхина</t>
+  </si>
+  <si>
+    <t>Белозуб Татьяна</t>
+  </si>
+  <si>
+    <t>Н. Петручук</t>
+  </si>
+  <si>
+    <t>Л. Петько</t>
+  </si>
+  <si>
+    <t>Т. Кузьмина</t>
+  </si>
+  <si>
+    <t>А. Гордеев</t>
+  </si>
+  <si>
+    <t>Марина Шрейнер</t>
+  </si>
+  <si>
+    <t>F.B.Holton</t>
+  </si>
+  <si>
+    <t>А. Эпп</t>
+  </si>
+  <si>
+    <t>М. Дешко</t>
+  </si>
+  <si>
+    <t>В. Гусакова</t>
+  </si>
+  <si>
+    <t>П. Цуман</t>
+  </si>
+  <si>
+    <t>А. Реймер</t>
+  </si>
+  <si>
+    <t>I. Шевченко</t>
+  </si>
+  <si>
+    <t>Ю. Мельник</t>
+  </si>
+  <si>
+    <t>П. Виртанен</t>
+  </si>
+  <si>
+    <t>А. Чепуренко</t>
+  </si>
+  <si>
+    <t>Т. Потаенко</t>
+  </si>
+  <si>
+    <t>Валерий Череванёв</t>
+  </si>
+  <si>
+    <t>Тимофей Коломийцев</t>
+  </si>
+  <si>
+    <t>James Rowe</t>
+  </si>
+  <si>
+    <t>Howard E. Smith</t>
+  </si>
+  <si>
+    <t>R. Lowry</t>
+  </si>
+  <si>
+    <t>С. Маген</t>
+  </si>
+  <si>
+    <t>аккорды</t>
+  </si>
+  <si>
+    <t>Д. Джулай</t>
+  </si>
+  <si>
+    <t>Вл. Горбачевский</t>
+  </si>
+  <si>
+    <t>Н. Крынец</t>
+  </si>
+  <si>
+    <t>О. Закусило</t>
+  </si>
+  <si>
+    <t>М. Концевич</t>
+  </si>
+  <si>
+    <t>В Петреченко</t>
+  </si>
+  <si>
+    <t>Eduard Ebel</t>
+  </si>
+  <si>
+    <t>Д. Весёлов</t>
+  </si>
+  <si>
+    <t>С. Василишин</t>
+  </si>
+  <si>
+    <t>А. Рыжов</t>
+  </si>
+  <si>
+    <t>Цуман Пётр</t>
+  </si>
+  <si>
+    <t>Таїса Устимчук</t>
+  </si>
+  <si>
+    <t>Павло Тумаш</t>
+  </si>
+  <si>
+    <t>С Тимохина</t>
+  </si>
+  <si>
+    <t>пер. В Яцюк</t>
+  </si>
+  <si>
+    <t>Дубовой Рувим</t>
+  </si>
+  <si>
+    <t>Мої джерела - у Христі (№35)</t>
+  </si>
+  <si>
+    <t>Ю. Рыжковой (Ю. Фирсовой)</t>
+  </si>
+  <si>
+    <t>Р Фот</t>
+  </si>
+  <si>
+    <t>Р. Ахметшин</t>
+  </si>
+  <si>
+    <t>Камерный - Р. Ахметшин</t>
+  </si>
+  <si>
+    <t>Матвеюк А М</t>
+  </si>
+  <si>
+    <t>Л. Камалова</t>
+  </si>
+  <si>
+    <t>В. Кривенков</t>
+  </si>
+  <si>
+    <t>гарм. Т. Козина</t>
+  </si>
+  <si>
+    <t>Т. Спесивцева</t>
+  </si>
+  <si>
+    <t>А Щеглов</t>
+  </si>
+  <si>
+    <t>А Эглит</t>
+  </si>
+  <si>
+    <t>Г Чайка</t>
+  </si>
+  <si>
+    <t>А Можаев</t>
+  </si>
+  <si>
+    <t>Г. Везикова</t>
+  </si>
+  <si>
+    <t>Л. Хархардина</t>
+  </si>
+  <si>
+    <t>Г. Винс</t>
+  </si>
+  <si>
+    <t>Гендель - арр. D. Clydesdale</t>
+  </si>
+  <si>
+    <t>В Стрелков</t>
+  </si>
+  <si>
+    <t>Д Махмуд-Оглы</t>
+  </si>
+  <si>
+    <t>Ch. Gabriel</t>
+  </si>
+  <si>
+    <t>Ю Богачов</t>
+  </si>
+  <si>
+    <t>А Краснокутский</t>
+  </si>
+  <si>
+    <t>С Горильчаник</t>
+  </si>
+  <si>
+    <t>В Б Мендруняк</t>
+  </si>
+  <si>
+    <t>Галина Самусь</t>
+  </si>
+  <si>
+    <t>И Крышко</t>
+  </si>
+  <si>
+    <t>Н. Шибких</t>
+  </si>
+  <si>
+    <t>А. Гапонюк</t>
+  </si>
+  <si>
+    <t>Ben Tevs</t>
+  </si>
+  <si>
+    <t>Г. Сегенчук</t>
+  </si>
+  <si>
+    <t>А. Шалимов</t>
+  </si>
+  <si>
+    <t>Л Н Курс</t>
+  </si>
+  <si>
+    <t>Э. Сковородко</t>
+  </si>
+  <si>
+    <t>Р.Коваленко</t>
+  </si>
+  <si>
+    <t>Г. Красненкова</t>
+  </si>
+  <si>
+    <t>А.И.Г.</t>
+  </si>
+  <si>
+    <t>Хор - обр. Гусакова</t>
+  </si>
+  <si>
+    <t>В.Ф. Миллер</t>
+  </si>
+  <si>
+    <t>Виталий Стрелков</t>
+  </si>
+  <si>
+    <t>Максим Ткаченко</t>
+  </si>
+  <si>
+    <t>Джерела №296</t>
+  </si>
+  <si>
+    <t>Л. Жидкова</t>
+  </si>
+  <si>
+    <t>А. Архангельский</t>
+  </si>
+  <si>
+    <t>Р. Бартмус</t>
+  </si>
+  <si>
+    <t>И. Проханов</t>
+  </si>
+  <si>
+    <t>Казаков</t>
+  </si>
+  <si>
+    <t>Духовой оркестр - арр. В.П.З.</t>
+  </si>
+  <si>
+    <t>Духовой оркестр 2</t>
+  </si>
+  <si>
+    <t>В. В. С.</t>
+  </si>
+  <si>
+    <t>I. Nichita</t>
+  </si>
+  <si>
+    <t>П. Чайковский</t>
+  </si>
+  <si>
+    <t>Л. Лазко</t>
+  </si>
+  <si>
+    <t>Т. Белозуб</t>
+  </si>
+  <si>
+    <t>Вокал 5-т</t>
+  </si>
+  <si>
+    <t>J. H. Johnston</t>
+  </si>
+  <si>
+    <t>D. B. Towner</t>
+  </si>
+  <si>
+    <t>Ксения Рындич</t>
+  </si>
+  <si>
+    <t>Духовой - инст. Заберезников</t>
+  </si>
+  <si>
+    <t>Духовой - В. Буду</t>
+  </si>
+  <si>
+    <t>Миди-оркестровки</t>
+  </si>
+  <si>
+    <t>аранж. Кенигсберг</t>
+  </si>
+  <si>
+    <t>В. М. Беличенко</t>
+  </si>
+  <si>
+    <t>Анс. НИ - J.B.</t>
+  </si>
+  <si>
+    <t>И. Кмета-Ефимович</t>
+  </si>
+  <si>
+    <t>С. Бычковский</t>
+  </si>
+  <si>
+    <t>Keith Getty</t>
+  </si>
+  <si>
+    <t>Kristyn Getty</t>
+  </si>
+  <si>
+    <t>Stuart Townend</t>
+  </si>
+  <si>
+    <t>С. Библенко</t>
+  </si>
+  <si>
+    <t>В Переверзев</t>
+  </si>
+  <si>
+    <t>В Иванов</t>
+  </si>
+  <si>
+    <t>Джерела №42</t>
+  </si>
+  <si>
+    <t>Василий Смирнов</t>
+  </si>
+  <si>
+    <t>Скр. 4-т - П. Румачик</t>
+  </si>
+  <si>
+    <t>Бандуры 2-т</t>
+  </si>
+  <si>
+    <t>Соло - украинский вариант</t>
+  </si>
+  <si>
+    <t>Смешанный орк. А Дрибноход</t>
+  </si>
+  <si>
+    <t>ПВ - 286</t>
+  </si>
+  <si>
+    <t>ПВ - 449 (541)</t>
+  </si>
+  <si>
+    <t>E. R. Latta</t>
+  </si>
+  <si>
+    <t>H. S. Perkins</t>
+  </si>
+  <si>
+    <t>ПВ 592 (692)</t>
+  </si>
+  <si>
+    <t>M. Bruce</t>
+  </si>
+  <si>
+    <t>L. Mason</t>
+  </si>
+  <si>
+    <t>Любовь Бледных</t>
+  </si>
+  <si>
+    <t>А. Фефелов</t>
+  </si>
+  <si>
+    <t>С. Горецкий</t>
+  </si>
+  <si>
+    <t>Соло и фортепиано</t>
+  </si>
+  <si>
+    <t>ЮИ - 25</t>
+  </si>
+  <si>
+    <t>Н. Водневский</t>
+  </si>
+  <si>
+    <t>Три разные мелодии</t>
+  </si>
+  <si>
+    <t>Г.С.</t>
+  </si>
+  <si>
+    <t>Донцов Константин</t>
+  </si>
+  <si>
+    <t>А. Рогальский</t>
+  </si>
+  <si>
+    <t>ОРНИ - Л. Петько</t>
+  </si>
+  <si>
+    <t>С Бас</t>
+  </si>
+  <si>
+    <t>Евгений Дмитриев</t>
+  </si>
+  <si>
+    <t>Петр Олийник</t>
+  </si>
+  <si>
+    <t>А. Мазалова</t>
+  </si>
+  <si>
+    <t>В. Скумбин</t>
+  </si>
+  <si>
+    <t>Т. Белицкая</t>
+  </si>
+  <si>
+    <t>Л. Тимченко</t>
+  </si>
+  <si>
+    <t>В. Згодько</t>
+  </si>
+  <si>
+    <t>Синди Берри</t>
+  </si>
+  <si>
+    <t>Л. Конкина</t>
+  </si>
+  <si>
+    <t>Л. Межохина</t>
+  </si>
+  <si>
+    <t>В. Дик</t>
+  </si>
+  <si>
+    <t>Л. Конкина - инстр. Парафейник</t>
+  </si>
+  <si>
+    <t>П.А. Вяземский</t>
+  </si>
+  <si>
+    <t>Е. К.</t>
+  </si>
+  <si>
+    <t>А. Ахметшина</t>
+  </si>
+  <si>
+    <t>Гусакова В.И.</t>
+  </si>
+  <si>
+    <t>О. Жидулов</t>
+  </si>
+  <si>
+    <t>Юлия Агапова</t>
+  </si>
+  <si>
+    <t>Н. Ломако</t>
+  </si>
+  <si>
+    <t>Валерий Квасневский</t>
+  </si>
+  <si>
+    <t>Ф. Мендельсон</t>
+  </si>
+  <si>
+    <t>Георгий Топал</t>
+  </si>
+  <si>
+    <t>Sally DeFord</t>
+  </si>
+  <si>
+    <t>С. Зайцева</t>
+  </si>
+  <si>
+    <t>А. Страделла</t>
+  </si>
+  <si>
+    <t>П. І. Олійник</t>
+  </si>
+  <si>
+    <t>Марія Гатала-Квасневська</t>
+  </si>
+  <si>
+    <t>Шумейко М.</t>
+  </si>
+  <si>
+    <t>П. Бальжик</t>
+  </si>
+  <si>
+    <t>Д. Мартынс</t>
+  </si>
+  <si>
+    <t>Ю. Хазарова</t>
+  </si>
+  <si>
+    <t>И. Скирда</t>
+  </si>
+  <si>
+    <t>Ирина Крышко</t>
+  </si>
+  <si>
+    <t>Ю. Костюк</t>
+  </si>
+  <si>
+    <t>О. Свистун</t>
+  </si>
+  <si>
+    <t>W.W.Walford</t>
+  </si>
+  <si>
+    <t>W.B.Bradbury</t>
+  </si>
+  <si>
+    <t>И. Шевченко</t>
   </si>
 </sst>
 </file>
@@ -694,10 +1426,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:G234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
+      <selection activeCell="E197" sqref="E197:E234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -705,11 +1437,13 @@
     <col min="1" max="1" width="26.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" customWidth="1"/>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -720,16 +1454,19 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G1" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -740,10 +1477,19 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -754,10 +1500,16 @@
         <v>49</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+      <c r="E3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -768,10 +1520,16 @@
         <v>50</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+      <c r="E4" t="s">
+        <v>121</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -782,10 +1540,16 @@
         <v>51</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+      <c r="E5" t="s">
+        <v>122</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -796,10 +1560,16 @@
         <v>52</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+      <c r="E6" t="s">
+        <v>123</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -809,9 +1579,17 @@
       <c r="C7" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" t="s">
+        <v>124</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -821,9 +1599,17 @@
       <c r="C8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D8" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" t="s">
+        <v>125</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -833,9 +1619,17 @@
       <c r="C9" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -845,9 +1639,14 @@
       <c r="C10" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D10" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -857,103 +1656,132 @@
       <c r="C11" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D11" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>58</v>
       </c>
       <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>59</v>
       </c>
       <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>60</v>
       </c>
       <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>62</v>
       </c>
       <c r="D16" s="2"/>
+      <c r="E16" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>63</v>
       </c>
       <c r="D17" s="2"/>
+      <c r="E17" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>64</v>
       </c>
       <c r="D18" s="2"/>
+      <c r="E18" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>65</v>
       </c>
       <c r="D19" s="2"/>
+      <c r="E19" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
@@ -966,38 +1794,51 @@
         <v>66</v>
       </c>
       <c r="D20" s="2"/>
+      <c r="E20" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D21" s="2"/>
+      <c r="E21" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="22" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="3"/>
+      <c r="B22" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="C22" s="2" t="s">
         <v>68</v>
       </c>
       <c r="D22" s="2"/>
+      <c r="E22" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="23" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="3"/>
       <c r="C23" s="2" t="s">
         <v>69</v>
       </c>
       <c r="D23" s="2"/>
+      <c r="E23" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="24" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
@@ -1008,6 +1849,9 @@
         <v>70</v>
       </c>
       <c r="D24" s="2"/>
+      <c r="E24" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="25" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
@@ -1018,6 +1862,9 @@
         <v>71</v>
       </c>
       <c r="D25" s="2"/>
+      <c r="E25" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="26" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
@@ -1028,6 +1875,9 @@
         <v>72</v>
       </c>
       <c r="D26" s="2"/>
+      <c r="E26" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="27" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
@@ -1038,6 +1888,9 @@
         <v>73</v>
       </c>
       <c r="D27" s="2"/>
+      <c r="E27" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="28" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
@@ -1045,9 +1898,12 @@
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D28" s="2"/>
+      <c r="E28" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
@@ -1058,6 +1914,9 @@
         <v>74</v>
       </c>
       <c r="D29" s="2"/>
+      <c r="E29" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
@@ -1068,6 +1927,9 @@
         <v>75</v>
       </c>
       <c r="D30" s="2"/>
+      <c r="E30" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
@@ -1078,6 +1940,9 @@
         <v>76</v>
       </c>
       <c r="D31" s="2"/>
+      <c r="E31" t="s">
+        <v>148</v>
+      </c>
       <c r="F31" s="3"/>
     </row>
     <row r="32" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1089,10 +1954,10 @@
         <v>77</v>
       </c>
       <c r="D32" s="2"/>
-      <c r="F32" s="3" t="str">
-        <f t="shared" ref="F32:F38" si="0">MID(E32,2,LEN(E32))</f>
-        <v/>
-      </c>
+      <c r="E32" t="s">
+        <v>149</v>
+      </c>
+      <c r="F32" s="3"/>
     </row>
     <row r="33" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
@@ -1103,10 +1968,10 @@
         <v>78</v>
       </c>
       <c r="D33" s="2"/>
-      <c r="F33" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="E33" t="s">
+        <v>150</v>
+      </c>
+      <c r="F33" s="3"/>
     </row>
     <row r="34" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
@@ -1117,10 +1982,10 @@
         <v>79</v>
       </c>
       <c r="D34" s="2"/>
-      <c r="F34" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="E34" t="s">
+        <v>151</v>
+      </c>
+      <c r="F34" s="3"/>
     </row>
     <row r="35" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
@@ -1128,52 +1993,1030 @@
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="2" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="D35" s="2"/>
-      <c r="F35" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="E35" t="s">
+        <v>152</v>
+      </c>
+      <c r="F35" s="3"/>
     </row>
     <row r="36" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D36" s="2"/>
-      <c r="F36" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="E36" t="s">
+        <v>153</v>
+      </c>
+      <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C37" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F37" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="E37" t="s">
+        <v>154</v>
+      </c>
+      <c r="F37" s="3"/>
     </row>
     <row r="38" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C38" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F38" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="E38" t="s">
+        <v>155</v>
+      </c>
+      <c r="F38" s="3"/>
     </row>
     <row r="39" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C39" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F39" s="3" t="str">
-        <f>MID(E39,2,LEN(E39))</f>
-        <v/>
+        <v>109</v>
+      </c>
+      <c r="E39" t="s">
+        <v>156</v>
+      </c>
+      <c r="F39" s="3"/>
+    </row>
+    <row r="40" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C40" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E40" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E41" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E42" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E43" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E44" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E45" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E46" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E47" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E48" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="49" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E49" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="50" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E50" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="51" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E51" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="52" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E52" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="53" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E53" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="54" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E54" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="55" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E55" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="56" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E56" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="57" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E57" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="58" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E58" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="59" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E59" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="60" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E60" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="61" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E61" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="62" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E62" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="63" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E63" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="64" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E64" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="65" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E65" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="66" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E66" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="67" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E67" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="68" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E68" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="69" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E69" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="70" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E70" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="71" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E71" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="72" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E72" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="73" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E73" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="74" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E74" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="75" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E75" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="76" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E76" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="77" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E77" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="78" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E78" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="79" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E79" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="80" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E80" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="81" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E81" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="82" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E82" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="83" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E83" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="84" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E84" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="85" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E85" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="86" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E86" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="87" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E87" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="88" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E88" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="89" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E89" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="90" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E90" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="91" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E91" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="92" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E92" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="93" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E93" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="94" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E94" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="95" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E95" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="96" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E96" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="97" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E97" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="98" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E98" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="99" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E99" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="100" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E100" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="101" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E101" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="102" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E102" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="103" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E103" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="104" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E104" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="105" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E105" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="106" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E106" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="107" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E107" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="108" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E108" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="109" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E109" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="110" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E110" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="111" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E111" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="112" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E112" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="113" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E113" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="114" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E114" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="115" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E115" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="116" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E116" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="117" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E117" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="118" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E118" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="119" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E119" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="120" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E120" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="121" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E121" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="122" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E122" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="123" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E123" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="124" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E124" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="125" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E125" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="126" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E126" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="127" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E127" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="128" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E128" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="129" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E129" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="130" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E130" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="131" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E131" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="132" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E132" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="133" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E133" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="134" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E134" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="135" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E135" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="136" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E136" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="137" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E137" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="138" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E138" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="139" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E139" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="140" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E140" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="141" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E141" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="142" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E142" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="143" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E143" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="144" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E144" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="145" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E145" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="146" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E146" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="147" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E147" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="148" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E148" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="149" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E149" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="150" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E150" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="151" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E151" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="152" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E152" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="153" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E153" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="154" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E154" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="155" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E155" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="156" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E156" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="157" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E157" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="158" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E158" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="159" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E159" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="160" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E160" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="161" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E161" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="162" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E162" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="163" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E163" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="164" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E164" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="165" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E165" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="166" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E166" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="167" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E167" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="168" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E168" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="169" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E169" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="170" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E170" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="171" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E171" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="172" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E172" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="173" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E173" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="174" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E174" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="175" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E175" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="176" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E176" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="177" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E177" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="178" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E178" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="179" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E179" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="180" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E180" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="181" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E181" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="182" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E182" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="183" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E183" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="184" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E184" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="185" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E185" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="186" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E186" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="187" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E187" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="188" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E188" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="189" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E189" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="190" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E190" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="191" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E191" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="192" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E192" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="193" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E193" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="194" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E194" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="195" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E195" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="196" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E196" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="197" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E197" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="198" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E198" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="199" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E199" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="200" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E200" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="201" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E201" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="202" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E202" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="203" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E203" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="204" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E204" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="205" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E205" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="206" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E206" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="207" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E207" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="208" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E208" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="209" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E209" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="210" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E210" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="211" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E211" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="212" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E212" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="213" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E213" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="214" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E214" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="215" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E215" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="216" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E216" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="217" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E217" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="218" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E218" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="219" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E219" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="220" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E220" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="221" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E221" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="222" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E222" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="223" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E223" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="224" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E224" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="225" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E225" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="226" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E226" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="227" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E227" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="228" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E228" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="229" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E229" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="230" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E230" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="231" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E231" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="232" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E232" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="233" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E233" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="234" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E234" t="s">
+        <v>347</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lots of works done for normazliation and updating the index
</commit_message>
<xml_diff>
--- a/1.Webscraper/Index.xlsx
+++ b/1.Webscraper/Index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikol\Noty-Database\1.Webscraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCFCD0E-7B0D-4636-9231-5CFB37887671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4B56AD1-8D90-4B2B-91C2-4FDCA73F346E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="362">
   <si>
     <t>Categories/Occasions</t>
   </si>
@@ -225,9 +225,6 @@
     <t>Ансамбль НИ</t>
   </si>
   <si>
-    <t>Аккордеон - баян</t>
-  </si>
-  <si>
     <t>Бандура</t>
   </si>
   <si>
@@ -372,12 +369,6 @@
     <t>Трубы 2-т</t>
   </si>
   <si>
-    <t>3-o - English</t>
-  </si>
-  <si>
-    <t>3-о - Русский</t>
-  </si>
-  <si>
     <t>Хор - русский вариант</t>
   </si>
   <si>
@@ -1084,6 +1075,57 @@
   </si>
   <si>
     <t>И. Шевченко</t>
+  </si>
+  <si>
+    <t>Миди аранжировки</t>
+  </si>
+  <si>
+    <t>3-o English</t>
+  </si>
+  <si>
+    <t>3-о Русский</t>
+  </si>
+  <si>
+    <t>Аккордеон</t>
+  </si>
+  <si>
+    <t>Баян</t>
+  </si>
+  <si>
+    <t>На латышском языке</t>
+  </si>
+  <si>
+    <t>Хор + трио</t>
+  </si>
+  <si>
+    <t>Євангельскі Пісні</t>
+  </si>
+  <si>
+    <t>4 флейты</t>
+  </si>
+  <si>
+    <t>Утро Жизни</t>
+  </si>
+  <si>
+    <t>Джерела</t>
+  </si>
+  <si>
+    <t>Колядка</t>
+  </si>
+  <si>
+    <t>Песни для детей</t>
+  </si>
+  <si>
+    <t>ПВ</t>
+  </si>
+  <si>
+    <t>Прекрасный удел</t>
+  </si>
+  <si>
+    <t>Гусли</t>
+  </si>
+  <si>
+    <t>Гимны Христиан</t>
   </si>
 </sst>
 </file>
@@ -1428,8 +1470,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
-      <selection activeCell="E197" sqref="E197:E234"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1439,7 +1481,7 @@
     <col min="3" max="3" width="19.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1454,16 +1496,16 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1477,16 +1519,16 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1500,13 +1542,16 @@
         <v>49</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E3" t="s">
-        <v>120</v>
+        <v>117</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>352</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1520,13 +1565,16 @@
         <v>50</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E4" t="s">
-        <v>121</v>
+        <v>118</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>354</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>110</v>
+        <v>346</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1540,13 +1588,16 @@
         <v>51</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E5" t="s">
-        <v>122</v>
+        <v>119</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>355</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>111</v>
+        <v>347</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1560,13 +1611,16 @@
         <v>52</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E6" t="s">
-        <v>123</v>
+        <v>120</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>358</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1580,13 +1634,16 @@
         <v>53</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E7" t="s">
-        <v>124</v>
+        <v>121</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>359</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1600,13 +1657,16 @@
         <v>54</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E8" t="s">
-        <v>125</v>
+        <v>122</v>
+      </c>
+      <c r="F8" t="s">
+        <v>360</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1620,13 +1680,16 @@
         <v>55</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E9" t="s">
-        <v>126</v>
+        <v>123</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>361</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1640,10 +1703,13 @@
         <v>56</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E10" t="s">
-        <v>127</v>
+        <v>124</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1657,10 +1723,10 @@
         <v>57</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E11" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1668,14 +1734,16 @@
         <v>19</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>345</v>
+      </c>
       <c r="E12" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1683,14 +1751,14 @@
         <v>20</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>59</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1698,14 +1766,14 @@
         <v>21</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>60</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1713,14 +1781,14 @@
         <v>22</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>61</v>
+        <v>348</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1728,14 +1796,14 @@
         <v>23</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1743,14 +1811,14 @@
         <v>24</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1758,14 +1826,14 @@
         <v>25</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1773,14 +1841,14 @@
         <v>26</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1788,14 +1856,14 @@
         <v>27</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1803,14 +1871,14 @@
         <v>28</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1818,26 +1886,29 @@
         <v>29</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>30</v>
       </c>
+      <c r="B23" s="3" t="s">
+        <v>351</v>
+      </c>
       <c r="C23" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1846,11 +1917,11 @@
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1859,11 +1930,11 @@
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1872,11 +1943,11 @@
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1885,11 +1956,11 @@
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1898,11 +1969,11 @@
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1911,11 +1982,11 @@
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1924,11 +1995,11 @@
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1937,11 +2008,11 @@
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F31" s="3"/>
     </row>
@@ -1951,11 +2022,11 @@
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F32" s="3"/>
     </row>
@@ -1965,11 +2036,11 @@
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F33" s="3"/>
     </row>
@@ -1979,11 +2050,11 @@
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F34" s="3"/>
     </row>
@@ -1993,11 +2064,11 @@
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F35" s="3"/>
     </row>
@@ -2006,1017 +2077,1029 @@
         <v>39</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
+        <v>356</v>
+      </c>
       <c r="C37" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E37" t="s">
+        <v>151</v>
+      </c>
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E37" t="s">
-        <v>154</v>
-      </c>
-      <c r="F37" s="3"/>
-    </row>
-    <row r="38" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C38" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="E38" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F38" s="3"/>
     </row>
     <row r="39" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C39" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E39" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F39" s="3"/>
     </row>
     <row r="40" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C40" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E40" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C41" s="2" t="s">
+        <v>349</v>
+      </c>
       <c r="E41" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C42" s="2" t="s">
+        <v>353</v>
+      </c>
       <c r="E42" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E43" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E44" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E45" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E46" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E47" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E48" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="49" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E49" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="50" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E50" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="51" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E51" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="52" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E52" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="53" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E53" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="54" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E54" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="55" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E55" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="56" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E56" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="57" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E57" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="58" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E58" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="59" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E59" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="60" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E60" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="61" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E61" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="62" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E62" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="63" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E63" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="64" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E64" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="65" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E65" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="66" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E66" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="67" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E67" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="68" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E68" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="69" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E69" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="70" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E70" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="71" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E71" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="72" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E72" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="73" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E73" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="74" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E74" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="75" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E75" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="76" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E76" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="77" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E77" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="78" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E78" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="79" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E79" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="80" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E80" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="81" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E81" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="82" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E82" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="83" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E83" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="84" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E84" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="85" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E85" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="86" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E86" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="87" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E87" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="88" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E88" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="89" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E89" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="90" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E90" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="91" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E91" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="92" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E92" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="93" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E93" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="94" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E94" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="95" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E95" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="96" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E96" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="97" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E97" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="98" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E98" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="99" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E99" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="100" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E100" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="101" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E101" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="102" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E102" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="103" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E103" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="104" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E104" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="105" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E105" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="106" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E106" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="107" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E107" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="108" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E108" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="109" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E109" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="110" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E110" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="111" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E111" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="112" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E112" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="113" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E113" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="114" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E114" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="115" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E115" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="116" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E116" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="117" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E117" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="118" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E118" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="119" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E119" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="120" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E120" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="121" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E121" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="122" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E122" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="123" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E123" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="124" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E124" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="125" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E125" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="126" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E126" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="127" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E127" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="128" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E128" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="129" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E129" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="130" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E130" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="131" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E131" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="132" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E132" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="133" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E133" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="134" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E134" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="135" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E135" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="136" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E136" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="137" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E137" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="138" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E138" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="139" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E139" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="140" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E140" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="141" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E141" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="142" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E142" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="143" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E143" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="144" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E144" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="145" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E145" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="146" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E146" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="147" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E147" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="148" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E148" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="149" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E149" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="150" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E150" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="151" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E151" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="152" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E152" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="153" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E153" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="154" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E154" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="155" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E155" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="156" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E156" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="157" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E157" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="158" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E158" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="159" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E159" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="160" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E160" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="161" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E161" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="162" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E162" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="163" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E163" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="164" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E164" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="165" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E165" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="166" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E166" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="167" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E167" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="168" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E168" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="169" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E169" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="170" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E170" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="171" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E171" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="172" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E172" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="173" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E173" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="174" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E174" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="175" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E175" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="176" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E176" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="177" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E177" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="178" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E178" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="179" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E179" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="180" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E180" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="181" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E181" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="182" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E182" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="183" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E183" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="184" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E184" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="185" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E185" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="186" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E186" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="187" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E187" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="188" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E188" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="189" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E189" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="190" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E190" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="191" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E191" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="192" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E192" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="193" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E193" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="194" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E194" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="195" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E195" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="196" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E196" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="197" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E197" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="198" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E198" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="199" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E199" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="200" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E200" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="201" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E201" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="202" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E202" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="203" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E203" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="204" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E204" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="205" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E205" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="206" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E206" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="207" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E207" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="208" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E208" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="209" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E209" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="210" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E210" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="211" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E211" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="212" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E212" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="213" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E213" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="214" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E214" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="215" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E215" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="216" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E216" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="217" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E217" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="218" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E218" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="219" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E219" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="220" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E220" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="221" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E221" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="222" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E222" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="223" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E223" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="224" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E224" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="225" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E225" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="226" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E226" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="227" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E227" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="228" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E228" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="229" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E229" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="230" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E230" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="231" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E231" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="232" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E232" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="233" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E233" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="234" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E234" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Database files and roughly finished implmenting the sqlite3 database
</commit_message>
<xml_diff>
--- a/1.Webscraper/Index.xlsx
+++ b/1.Webscraper/Index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikol\Noty-Database\1.Webscraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D9CA31-8571-4465-A92C-AB30AD8DAD25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580CD1C1-9DBF-4FA7-A25D-5D58FC73EA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="735">
   <si>
     <t>Categories/Occasions</t>
   </si>
@@ -633,9 +633,6 @@
     <t>Том Феттке</t>
   </si>
   <si>
-    <t>SamuelVulcan Mary</t>
-  </si>
-  <si>
     <t>Perebicovschi S.</t>
   </si>
   <si>
@@ -2230,6 +2227,24 @@
   </si>
   <si>
     <t>русский вариант</t>
+  </si>
+  <si>
+    <t>М Шрейнер</t>
+  </si>
+  <si>
+    <t>Traducere A. Daranuța</t>
+  </si>
+  <si>
+    <t>Samuel Heatwole and D. Bauman</t>
+  </si>
+  <si>
+    <t>Graham Kendrick</t>
+  </si>
+  <si>
+    <t>Vulcan Mary</t>
+  </si>
+  <si>
+    <t>В. Буду</t>
   </si>
 </sst>
 </file>
@@ -2284,13 +2299,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2572,10 +2588,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G638"/>
+  <dimension ref="A1:G643"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2810,7 +2826,7 @@
         <v>114</v>
       </c>
       <c r="E10" t="s">
-        <v>197</v>
+        <v>733</v>
       </c>
       <c r="F10" t="s">
         <v>147</v>
@@ -2833,7 +2849,7 @@
         <v>121</v>
       </c>
       <c r="E11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>149</v>
@@ -2862,14 +2878,14 @@
         <v>151</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>81</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -2882,14 +2898,14 @@
         <v>179</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>82</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -2899,17 +2915,17 @@
         <v>144</v>
       </c>
       <c r="E14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F14" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>83</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -2919,17 +2935,17 @@
         <v>148</v>
       </c>
       <c r="E15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F15" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>84</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -2942,14 +2958,14 @@
         <v>180</v>
       </c>
       <c r="F16" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>85</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -2969,7 +2985,7 @@
       <c r="A18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="4" t="s">
         <v>90</v>
       </c>
       <c r="C18" t="s">
@@ -2979,37 +2995,37 @@
         <v>154</v>
       </c>
       <c r="E18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F18" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="4" t="s">
         <v>91</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>62</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>93</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -3019,48 +3035,48 @@
         <v>176</v>
       </c>
       <c r="E20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>102</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>64</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="E21" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="4" t="s">
         <v>113</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>65</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="E22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="4" t="s">
         <v>131</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -3068,7 +3084,7 @@
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3081,7 +3097,7 @@
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3146,7 +3162,7 @@
       </c>
       <c r="D29" s="2"/>
       <c r="E29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3159,7 +3175,7 @@
       </c>
       <c r="D30" s="2"/>
       <c r="E30" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3172,7 +3188,7 @@
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F31" s="3"/>
     </row>
@@ -3186,7 +3202,7 @@
       </c>
       <c r="D32" s="2"/>
       <c r="E32" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F32" s="3"/>
     </row>
@@ -3200,7 +3216,7 @@
       </c>
       <c r="D33" s="2"/>
       <c r="E33" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F33" s="3"/>
     </row>
@@ -3228,7 +3244,7 @@
       </c>
       <c r="D35" s="2"/>
       <c r="E35" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F35" s="3"/>
     </row>
@@ -3241,7 +3257,7 @@
       </c>
       <c r="D36" s="2"/>
       <c r="E36" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F36" s="3"/>
     </row>
@@ -3277,7 +3293,7 @@
         <v>97</v>
       </c>
       <c r="E39" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F39" s="3"/>
     </row>
@@ -3289,7 +3305,7 @@
         <v>98</v>
       </c>
       <c r="E40" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3300,7 +3316,7 @@
         <v>108</v>
       </c>
       <c r="E41" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3308,7 +3324,7 @@
         <v>110</v>
       </c>
       <c r="E42" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3316,7 +3332,7 @@
         <v>129</v>
       </c>
       <c r="E43" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3324,7 +3340,7 @@
         <v>133</v>
       </c>
       <c r="E44" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3332,7 +3348,7 @@
         <v>146</v>
       </c>
       <c r="E45" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3340,7 +3356,7 @@
         <v>156</v>
       </c>
       <c r="E46" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3353,30 +3369,30 @@
     </row>
     <row r="48" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C48" s="2" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E48" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="49" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E49" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="50" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="51" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E51" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="52" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E52" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="53" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3386,52 +3402,52 @@
     </row>
     <row r="54" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E54" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="55" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E55" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="56" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E56" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="57" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E57" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="58" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E58" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="59" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E59" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="60" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E60" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="61" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E61" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="62" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E62" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="63" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E63" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="64" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3446,22 +3462,22 @@
     </row>
     <row r="66" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E66" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="67" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E67" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="68" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E68" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="69" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E69" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="70" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3486,67 +3502,67 @@
     </row>
     <row r="74" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E74" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="75" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E75" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="76" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E76" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="77" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E77" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="78" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E78" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="79" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E79" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="80" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E80" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="81" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E81" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="82" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E82" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="83" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E83" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="84" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E84" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="85" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E85" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="86" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E86" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="87" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3571,17 +3587,17 @@
     </row>
     <row r="91" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E91" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="92" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E92" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="93" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E93" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="94" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3601,52 +3617,52 @@
     </row>
     <row r="97" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E97" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="98" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E98" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="99" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E99" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="100" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E100" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="101" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E101" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="102" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E102" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="103" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E103" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="104" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E104" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="105" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E105" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="106" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E106" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="107" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3656,22 +3672,22 @@
     </row>
     <row r="108" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E108" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="109" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E109" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="110" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E110" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="111" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E111" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="112" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3681,37 +3697,37 @@
     </row>
     <row r="113" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E113" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="114" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E114" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="115" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E115" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="116" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E116" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="117" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E117" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="118" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E118" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="119" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E119" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="120" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3721,22 +3737,22 @@
     </row>
     <row r="121" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E121" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="122" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E122" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="123" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E123" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="124" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E124" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="125" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3746,117 +3762,117 @@
     </row>
     <row r="126" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E126" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="127" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E127" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="128" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E128" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="129" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E129" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="130" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E130" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="131" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E131" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="132" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E132" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="133" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E133" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="134" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E134" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="135" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E135" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="136" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E136" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="137" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E137" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="138" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E138" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="139" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E139" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="140" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E140" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="141" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E141" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="142" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E142" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="143" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E143" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="144" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E144" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="145" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E145" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="146" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E146" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="147" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E147" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="148" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E148" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="149" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3866,302 +3882,302 @@
     </row>
     <row r="150" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E150" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="151" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E151" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="152" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E152" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="153" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E153" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="154" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E154" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="155" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E155" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="156" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E156" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="157" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E157" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="158" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E158" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="159" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E159" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="160" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E160" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="161" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E161" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="162" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E162" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="163" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E163" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="164" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E164" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="165" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E165" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="166" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E166" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="167" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E167" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="168" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E168" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="169" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E169" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="170" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E170" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="171" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E171" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="172" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E172" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="173" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E173" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="174" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E174" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="175" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E175" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="176" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E176" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="177" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E177" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="178" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E178" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="179" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E179" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="180" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E180" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="181" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E181" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="182" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E182" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="183" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E183" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="184" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E184" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="185" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E185" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="186" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E186" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="187" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E187" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="188" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E188" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="189" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E189" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="190" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E190" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="191" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E191" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="192" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E192" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="193" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E193" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="194" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E194" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="195" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E195" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="196" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E196" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="197" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E197" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="198" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E198" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="199" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E199" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="200" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E200" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="201" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E201" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="202" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E202" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="203" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E203" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="204" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E204" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="205" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E205" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="206" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E206" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="207" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E207" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="208" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E208" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="209" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E209" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="210" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4171,272 +4187,272 @@
     </row>
     <row r="211" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E211" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="212" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E212" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="213" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E213" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="214" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E214" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="215" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E215" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="216" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E216" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="217" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E217" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="218" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E218" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="219" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E219" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="220" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E220" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="221" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E221" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="222" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E222" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="223" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E223" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="224" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E224" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="225" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E225" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="226" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E226" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="227" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E227" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="228" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E228" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="229" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E229" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="230" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E230" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="231" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E231" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="232" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E232" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="233" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E233" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="234" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E234" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="235" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E235" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="236" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E236" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="237" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E237" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="238" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E238" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="239" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E239" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="240" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E240" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="241" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E241" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="242" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E242" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="243" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E243" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="244" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E244" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="245" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E245" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="246" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E246" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="247" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E247" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="248" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E248" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="249" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E249" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="250" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E250" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="251" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E251" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="252" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E252" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="253" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E253" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="254" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E254" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="255" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E255" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="256" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E256" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="257" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E257" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="258" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E258" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="259" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E259" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="260" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E260" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="261" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E261" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="262" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E262" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="263" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E263" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="264" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E264" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="265" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4446,247 +4462,247 @@
     </row>
     <row r="266" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E266" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="267" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E267" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="268" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E268" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="269" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E269" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="270" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E270" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="271" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E271" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="272" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E272" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="273" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E273" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="274" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E274" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="275" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E275" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="276" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E276" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="277" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E277" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="278" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E278" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="279" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E279" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="280" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E280" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="281" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E281" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="282" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E282" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="283" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E283" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="284" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E284" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="285" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E285" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="286" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E286" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="287" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E287" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="288" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E288" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="289" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E289" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="290" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E290" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="291" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E291" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="292" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E292" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="293" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E293" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="294" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E294" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="295" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E295" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="296" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E296" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="297" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E297" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="298" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E298" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="299" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E299" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="300" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E300" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="301" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E301" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="302" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E302" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="303" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E303" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="304" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E304" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="305" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E305" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="306" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E306" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="307" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E307" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="308" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E308" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="309" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E309" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="310" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E310" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="311" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E311" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="312" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E312" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="313" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E313" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="314" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E314" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="315" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4696,572 +4712,572 @@
     </row>
     <row r="316" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E316" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="317" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E317" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="318" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E318" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="319" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E319" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="320" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E320" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="321" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E321" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="322" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E322" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="323" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E323" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="324" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E324" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="325" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E325" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="326" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E326" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="327" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E327" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="328" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E328" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="329" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E329" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="330" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E330" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="331" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E331" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="332" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E332" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="333" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E333" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="334" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E334" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="335" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E335" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="336" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E336" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="337" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E337" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="338" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E338" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="339" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E339" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="340" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E340" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="341" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E341" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="342" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E342" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="343" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E343" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="344" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E344" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="345" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E345" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="346" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E346" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="347" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E347" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="348" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E348" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="349" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E349" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="350" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E350" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="351" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E351" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="352" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E352" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="353" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E353" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="354" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E354" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="355" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E355" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="356" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E356" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="357" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E357" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="358" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E358" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="359" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E359" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="360" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E360" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="361" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E361" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="362" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E362" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="363" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E363" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="364" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E364" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="365" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E365" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="366" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E366" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="367" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E367" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="368" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E368" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="369" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E369" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="370" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E370" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="371" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E371" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="372" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E372" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="373" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E373" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="374" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E374" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="375" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E375" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="376" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E376" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="377" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E377" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="378" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E378" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="379" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E379" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="380" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E380" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="381" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E381" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="382" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E382" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="383" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E383" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="384" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E384" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="385" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E385" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="386" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E386" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="387" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E387" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="388" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E388" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="389" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E389" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="390" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E390" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="391" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E391" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="392" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E392" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="393" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E393" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="394" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E394" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="395" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E395" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="396" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E396" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="397" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E397" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="398" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E398" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="399" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E399" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="400" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E400" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="401" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E401" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="402" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E402" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="403" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E403" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="404" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E404" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="405" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E405" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="406" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E406" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="407" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E407" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="408" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E408" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="409" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E409" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="410" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E410" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="411" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E411" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="412" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E412" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="413" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E413" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="414" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E414" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="415" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E415" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="416" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E416" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="417" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E417" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="418" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E418" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="419" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E419" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="420" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E420" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="421" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E421" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="422" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E422" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="423" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E423" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="424" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E424" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="425" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E425" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="426" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E426" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="427" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E427" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="428" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E428" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="429" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E429" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="430" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5271,107 +5287,107 @@
     </row>
     <row r="431" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E431" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="432" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E432" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="433" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E433" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="434" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E434" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="435" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E435" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="436" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E436" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="437" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E437" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="438" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E438" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="439" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E439" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="440" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E440" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="441" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E441" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="442" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E442" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="443" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E443" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="444" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E444" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="445" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E445" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="446" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E446" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="447" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E447" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="448" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E448" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="449" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E449" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="450" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E450" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="451" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E451" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="452" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5386,12 +5402,12 @@
     </row>
     <row r="454" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E454" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="455" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E455" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="456" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5401,87 +5417,87 @@
     </row>
     <row r="457" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E457" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="458" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E458" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="459" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E459" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="460" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E460" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="461" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E461" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="462" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E462" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="463" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E463" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="464" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E464" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="465" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E465" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="466" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E466" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="467" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E467" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="468" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E468" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="469" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E469" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="470" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E470" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="471" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E471" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="472" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E472" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="473" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E473" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="474" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5491,102 +5507,102 @@
     </row>
     <row r="475" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E475" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="476" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E476" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="477" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E477" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="478" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E478" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="479" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E479" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="480" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E480" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="481" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E481" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="482" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E482" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="483" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E483" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="484" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E484" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="485" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E485" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="486" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E486" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="487" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E487" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="488" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E488" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="489" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E489" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="490" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E490" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="491" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E491" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="492" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E492" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="493" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E493" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="494" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E494" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="495" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5596,87 +5612,87 @@
     </row>
     <row r="496" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E496" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="497" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E497" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="499" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E499" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="500" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E500" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="501" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E501" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="502" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E502" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="503" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E503" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="504" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E504" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="505" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E505" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="506" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E506" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="507" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E507" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="508" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E508" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="509" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E509" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="510" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E510" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="511" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E511" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="512" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E512" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="513" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E513" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="514" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5686,27 +5702,27 @@
     </row>
     <row r="515" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E515" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="516" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E516" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="517" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E517" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="518" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E518" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="519" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E519" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="520" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5716,327 +5732,327 @@
     </row>
     <row r="521" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E521" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="522" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E522" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="523" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E523" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="524" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E524" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="525" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E525" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="526" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E526" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="527" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E527" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="528" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E528" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="529" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E529" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="530" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E530" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="531" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E531" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="532" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E532" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="533" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E533" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="534" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E534" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="535" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E535" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="536" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E536" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="537" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E537" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="538" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E538" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="539" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E539" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="540" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E540" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="541" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E541" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="542" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E542" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="543" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E543" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="544" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E544" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="545" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E545" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="546" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E546" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="547" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E547" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="548" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E548" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="549" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E549" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="550" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E550" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="551" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E551" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="552" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E552" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="553" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E553" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="554" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E554" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="555" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E555" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="556" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E556" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="557" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E557" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="558" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E558" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="559" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E559" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="560" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E560" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="561" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E561" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="562" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E562" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="563" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E563" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="564" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E564" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="565" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E565" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="566" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E566" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="567" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E567" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="568" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E568" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="569" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E569" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="570" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E570" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="571" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E571" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="572" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E572" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="573" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E573" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="574" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E574" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="575" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E575" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="576" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E576" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="577" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E577" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="578" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E578" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="579" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E579" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="580" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E580" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="581" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E581" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="582" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E582" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="583" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E583" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="584" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E584" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="585" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E585" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="586" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6046,142 +6062,142 @@
     </row>
     <row r="587" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E587" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="588" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E588" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="589" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E589" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="590" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E590" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="591" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E591" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="592" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E592" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="593" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E593" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="594" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E594" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="595" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E595" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="596" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E596" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="597" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E597" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="598" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E598" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="599" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E599" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="600" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E600" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="601" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E601" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="602" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E602" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="603" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E603" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="604" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E604" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="605" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E605" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="606" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E606" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="607" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E607" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="608" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E608" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="609" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E609" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="610" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E610" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="611" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E611" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="612" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E612" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="613" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E613" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="614" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E614" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="615" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6196,112 +6212,137 @@
     </row>
     <row r="617" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E617" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="618" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E618" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="619" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E619" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="620" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E620" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="621" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E621" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="622" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E622" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="623" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E623" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="624" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E624" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="625" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E625" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="626" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E626" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="627" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E627" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="628" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E628" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="629" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E629" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="630" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E630" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="631" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E631" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="632" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E632" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="633" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E633" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="634" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E634" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="635" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E635" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="636" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E636" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="637" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E637" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="638" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E638" t="s">
-        <v>718</v>
+        <v>717</v>
+      </c>
+    </row>
+    <row r="639" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E639" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="640" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E640" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="641" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E641" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="642" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E642" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="643" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E643" t="s">
+        <v>734</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more SQL files
</commit_message>
<xml_diff>
--- a/1.Webscraper/Index.xlsx
+++ b/1.Webscraper/Index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikol\Noty-Database\1.Webscraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580CD1C1-9DBF-4FA7-A25D-5D58FC73EA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94478FF-6A1F-4726-B780-8AE1DE8217CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="735">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="736">
   <si>
     <t>Categories/Occasions</t>
   </si>
@@ -420,12 +420,6 @@
     <t>Миди аранжировки</t>
   </si>
   <si>
-    <t>3-o English</t>
-  </si>
-  <si>
-    <t>3-о Русский</t>
-  </si>
-  <si>
     <t>Аккордеон</t>
   </si>
   <si>
@@ -2245,6 +2239,15 @@
   </si>
   <si>
     <t>В. Буду</t>
+  </si>
+  <si>
+    <t>3-o - English</t>
+  </si>
+  <si>
+    <t>3-о - Русский</t>
+  </si>
+  <si>
+    <t>Razele cerului</t>
   </si>
 </sst>
 </file>
@@ -2588,10 +2591,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G643"/>
+  <dimension ref="A1:G644"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="C640" workbookViewId="0">
+      <selection activeCell="E648" sqref="E648"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2642,7 +2645,7 @@
         <v>87</v>
       </c>
       <c r="E2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>111</v>
@@ -2659,16 +2662,16 @@
         <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>88</v>
       </c>
       <c r="E3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>107</v>
@@ -2688,13 +2691,13 @@
         <v>89</v>
       </c>
       <c r="E4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>126</v>
+        <v>733</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2711,13 +2714,13 @@
         <v>95</v>
       </c>
       <c r="E5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>127</v>
+        <v>734</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2734,10 +2737,10 @@
         <v>100</v>
       </c>
       <c r="E6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>109</v>
@@ -2757,10 +2760,10 @@
         <v>101</v>
       </c>
       <c r="E7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>112</v>
@@ -2780,10 +2783,10 @@
         <v>103</v>
       </c>
       <c r="E8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>115</v>
@@ -2803,10 +2806,10 @@
         <v>104</v>
       </c>
       <c r="E9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>112</v>
@@ -2826,13 +2829,13 @@
         <v>114</v>
       </c>
       <c r="E10" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="F10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2849,13 +2852,13 @@
         <v>121</v>
       </c>
       <c r="E11" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2872,13 +2875,13 @@
         <v>125</v>
       </c>
       <c r="E12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2892,13 +2895,13 @@
         <v>58</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2912,13 +2915,13 @@
         <v>59</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F14" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2932,13 +2935,13 @@
         <v>60</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E15" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F15" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2949,16 +2952,16 @@
         <v>84</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E16" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F16" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2972,13 +2975,13 @@
         <v>61</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E17" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F17" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2989,16 +2992,16 @@
         <v>90</v>
       </c>
       <c r="C18" t="s">
+        <v>150</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>154</v>
-      </c>
       <c r="E18" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F18" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3012,13 +3015,13 @@
         <v>62</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3032,10 +3035,10 @@
         <v>63</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E20" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3049,10 +3052,10 @@
         <v>64</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="E21" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3066,10 +3069,10 @@
         <v>65</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="E22" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3077,14 +3080,14 @@
         <v>30</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>66</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3097,7 +3100,7 @@
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3110,7 +3113,7 @@
       </c>
       <c r="D25" s="2"/>
       <c r="E25" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3123,7 +3126,7 @@
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3136,7 +3139,7 @@
       </c>
       <c r="D27" s="2"/>
       <c r="E27" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3149,7 +3152,7 @@
       </c>
       <c r="D28" s="2"/>
       <c r="E28" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3162,7 +3165,7 @@
       </c>
       <c r="D29" s="2"/>
       <c r="E29" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3175,7 +3178,7 @@
       </c>
       <c r="D30" s="2"/>
       <c r="E30" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3188,7 +3191,7 @@
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F31" s="3"/>
     </row>
@@ -3202,7 +3205,7 @@
       </c>
       <c r="D32" s="2"/>
       <c r="E32" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F32" s="3"/>
     </row>
@@ -3216,7 +3219,7 @@
       </c>
       <c r="D33" s="2"/>
       <c r="E33" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F33" s="3"/>
     </row>
@@ -3230,7 +3233,7 @@
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F34" s="3"/>
     </row>
@@ -3244,7 +3247,7 @@
       </c>
       <c r="D35" s="2"/>
       <c r="E35" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F35" s="3"/>
     </row>
@@ -3257,43 +3260,43 @@
       </c>
       <c r="D36" s="2"/>
       <c r="E36" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>96</v>
       </c>
       <c r="E37" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F37" s="3"/>
     </row>
     <row r="38" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>92</v>
       </c>
       <c r="E38" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F38" s="3"/>
     </row>
     <row r="39" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>97</v>
       </c>
       <c r="E39" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F39" s="3"/>
     </row>
@@ -3305,18 +3308,18 @@
         <v>98</v>
       </c>
       <c r="E40" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>108</v>
       </c>
       <c r="E41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3324,410 +3327,410 @@
         <v>110</v>
       </c>
       <c r="E42" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C43" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E43" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C44" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E44" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C45" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E45" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C46" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E46" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C47" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E47" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C48" s="2" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="E48" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="49" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E49" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="50" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="51" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E51" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="52" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E52" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="53" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E53" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="54" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E54" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="55" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E55" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="56" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E56" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="57" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E57" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="58" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E58" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="59" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E59" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="60" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E60" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="61" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E61" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="62" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E62" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="63" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E63" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="64" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E64" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="65" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E65" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="66" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E66" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="67" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E67" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="68" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E68" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="69" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E69" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="70" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E70" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="71" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E71" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="72" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E72" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="73" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E73" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="74" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E74" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="75" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E75" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="76" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E76" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="77" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E77" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="78" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E78" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="79" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E79" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="80" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E80" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="81" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E81" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="82" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E82" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="83" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E83" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="84" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E84" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="85" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E85" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="86" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E86" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="87" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E87" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="88" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E88" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="89" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E89" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="90" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E90" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="91" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E91" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="92" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E92" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="93" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E93" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="94" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E94" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="95" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E95" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="96" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E96" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="97" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E97" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="98" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E98" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="99" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E99" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="100" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E100" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="101" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E101" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="102" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E102" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="103" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E103" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="104" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E104" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="105" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E105" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="106" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E106" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="107" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E107" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="108" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E108" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="109" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E109" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="110" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E110" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="111" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E111" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="112" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E112" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="113" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E113" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="114" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E114" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="115" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E115" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="116" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E116" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="117" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E117" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="118" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E118" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="119" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E119" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="120" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3737,447 +3740,447 @@
     </row>
     <row r="121" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E121" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="122" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E122" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="123" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E123" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="124" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E124" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="125" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E125" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="126" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E126" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="127" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E127" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="128" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E128" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="129" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E129" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="130" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E130" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="131" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E131" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="132" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E132" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="133" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E133" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="134" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E134" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="135" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E135" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="136" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E136" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="137" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E137" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="138" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E138" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="139" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E139" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="140" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E140" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="141" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E141" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="142" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E142" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="143" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E143" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="144" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E144" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="145" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E145" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="146" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E146" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="147" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E147" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="148" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E148" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="149" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E149" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="150" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E150" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="151" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E151" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="152" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E152" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="153" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E153" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="154" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E154" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="155" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E155" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="156" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E156" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="157" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E157" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="158" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E158" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="159" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E159" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="160" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E160" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="161" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E161" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="162" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E162" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="163" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E163" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="164" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E164" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="165" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E165" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="166" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E166" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="167" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E167" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="168" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E168" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="169" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E169" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="170" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E170" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="171" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E171" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="172" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E172" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="173" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E173" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="174" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E174" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="175" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E175" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="176" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E176" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="177" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E177" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="178" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E178" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="179" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E179" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="180" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E180" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="181" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E181" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="182" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E182" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="183" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E183" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="184" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E184" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="185" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E185" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="186" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E186" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="187" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E187" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="188" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E188" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="189" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E189" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="190" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E190" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="191" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E191" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="192" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E192" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="193" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E193" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="194" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E194" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="195" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E195" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="196" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E196" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="197" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E197" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="198" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E198" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="199" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E199" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="200" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E200" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="201" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E201" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="202" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E202" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="203" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E203" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="204" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E204" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="205" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E205" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="206" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E206" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="207" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E207" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="208" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E208" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="209" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E209" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="210" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4187,272 +4190,272 @@
     </row>
     <row r="211" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E211" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="212" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E212" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="213" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E213" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="214" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E214" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="215" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E215" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="216" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E216" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="217" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E217" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="218" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E218" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="219" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E219" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="220" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E220" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="221" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E221" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="222" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E222" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="223" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E223" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="224" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E224" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="225" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E225" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="226" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E226" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="227" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E227" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="228" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E228" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="229" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E229" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="230" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E230" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="231" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E231" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="232" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E232" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="233" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E233" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="234" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E234" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="235" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E235" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="236" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E236" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="237" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E237" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="238" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E238" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="239" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E239" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="240" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E240" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="241" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E241" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="242" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E242" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="243" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E243" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="244" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E244" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="245" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E245" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="246" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E246" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="247" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E247" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="248" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E248" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="249" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E249" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="250" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E250" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="251" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E251" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="252" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E252" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="253" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E253" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="254" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E254" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="255" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E255" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="256" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E256" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="257" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E257" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="258" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E258" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="259" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E259" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="260" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E260" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="261" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E261" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="262" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E262" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="263" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E263" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="264" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E264" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="265" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4462,822 +4465,822 @@
     </row>
     <row r="266" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E266" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="267" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E267" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="268" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E268" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="269" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E269" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="270" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E270" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="271" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E271" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="272" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E272" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="273" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E273" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="274" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E274" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="275" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E275" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="276" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E276" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="277" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E277" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="278" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E278" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="279" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E279" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="280" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E280" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="281" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E281" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="282" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E282" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="283" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E283" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="284" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E284" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="285" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E285" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="286" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E286" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="287" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E287" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="288" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E288" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="289" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E289" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="290" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E290" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="291" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E291" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="292" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E292" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="293" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E293" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="294" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E294" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="295" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E295" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="296" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E296" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="297" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E297" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="298" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E298" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="299" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E299" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="300" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E300" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="301" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E301" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="302" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E302" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="303" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E303" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="304" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E304" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="305" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E305" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="306" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E306" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="307" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E307" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="308" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E308" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="309" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E309" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="310" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E310" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="311" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E311" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="312" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E312" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="313" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E313" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="314" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E314" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="315" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E315" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="316" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E316" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="317" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E317" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="318" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E318" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="319" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E319" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="320" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E320" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="321" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E321" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="322" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E322" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="323" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E323" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="324" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E324" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="325" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E325" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="326" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E326" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="327" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E327" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="328" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E328" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="329" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E329" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="330" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E330" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="331" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E331" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="332" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E332" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="333" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E333" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="334" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E334" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="335" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E335" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="336" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E336" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="337" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E337" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="338" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E338" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="339" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E339" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="340" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E340" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="341" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E341" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="342" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E342" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="343" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E343" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="344" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E344" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="345" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E345" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="346" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E346" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="347" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E347" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="348" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E348" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="349" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E349" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="350" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E350" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="351" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E351" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="352" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E352" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="353" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E353" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="354" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E354" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="355" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E355" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="356" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E356" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="357" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E357" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="358" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E358" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="359" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E359" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="360" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E360" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="361" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E361" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="362" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E362" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="363" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E363" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="364" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E364" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="365" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E365" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="366" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E366" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="367" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E367" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="368" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E368" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="369" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E369" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="370" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E370" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="371" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E371" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="372" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E372" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="373" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E373" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="374" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E374" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="375" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E375" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="376" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E376" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="377" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E377" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="378" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E378" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="379" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E379" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="380" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E380" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="381" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E381" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="382" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E382" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="383" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E383" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="384" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E384" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="385" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E385" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="386" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E386" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="387" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E387" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="388" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E388" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="389" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E389" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="390" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E390" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="391" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E391" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="392" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E392" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="393" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E393" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="394" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E394" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="395" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E395" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="396" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E396" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="397" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E397" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="398" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E398" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="399" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E399" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="400" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E400" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="401" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E401" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="402" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E402" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="403" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E403" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="404" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E404" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="405" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E405" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="406" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E406" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="407" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E407" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="408" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E408" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="409" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E409" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="410" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E410" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="411" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E411" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="412" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E412" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="413" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E413" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="414" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E414" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="415" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E415" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="416" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E416" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="417" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E417" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="418" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E418" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="419" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E419" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="420" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E420" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="421" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E421" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="422" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E422" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="423" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E423" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="424" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E424" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="425" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E425" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="426" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E426" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="427" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E427" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="428" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E428" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="429" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E429" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="430" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5287,107 +5290,107 @@
     </row>
     <row r="431" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E431" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="432" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E432" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="433" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E433" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="434" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E434" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="435" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E435" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="436" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E436" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="437" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E437" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="438" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E438" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="439" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E439" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="440" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E440" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="441" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E441" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="442" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E442" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="443" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E443" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="444" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E444" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="445" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E445" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="446" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E446" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="447" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E447" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="448" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E448" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="449" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E449" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="450" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E450" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="451" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E451" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="452" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5402,102 +5405,102 @@
     </row>
     <row r="454" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E454" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="455" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E455" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="456" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E456" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="457" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E457" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="458" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E458" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="459" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E459" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="460" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E460" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="461" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E461" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="462" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E462" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="463" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E463" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="464" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E464" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="465" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E465" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="466" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E466" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="467" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E467" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="468" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E468" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="469" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E469" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="470" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E470" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="471" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E471" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="472" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E472" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="473" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E473" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="474" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5507,102 +5510,102 @@
     </row>
     <row r="475" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E475" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="476" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E476" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="477" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E477" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="478" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E478" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="479" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E479" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="480" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E480" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="481" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E481" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="482" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E482" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="483" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E483" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="484" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E484" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="485" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E485" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="486" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E486" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="487" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E487" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="488" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E488" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="489" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E489" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="490" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E490" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="491" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E491" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="492" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E492" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="493" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E493" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="494" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E494" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="495" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5612,87 +5615,87 @@
     </row>
     <row r="496" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E496" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="497" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E497" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="499" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E499" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="500" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E500" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="501" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E501" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="502" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E502" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="503" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E503" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="504" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E504" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
     <row r="505" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E505" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
     </row>
     <row r="506" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E506" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="507" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E507" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
     </row>
     <row r="508" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E508" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="509" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E509" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
     </row>
     <row r="510" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E510" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="511" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E511" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
     </row>
     <row r="512" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E512" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="513" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E513" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
     <row r="514" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5702,27 +5705,27 @@
     </row>
     <row r="515" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E515" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
     </row>
     <row r="516" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E516" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="517" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E517" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
     <row r="518" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E518" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
     </row>
     <row r="519" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E519" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="520" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5732,327 +5735,327 @@
     </row>
     <row r="521" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E521" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="522" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E522" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
     </row>
     <row r="523" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E523" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="524" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E524" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="525" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E525" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="526" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E526" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="527" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E527" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="528" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E528" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="529" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E529" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="530" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E530" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="531" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E531" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="532" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E532" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="533" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E533" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="534" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E534" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="535" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E535" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="536" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E536" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="537" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E537" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="538" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E538" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="539" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E539" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="540" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E540" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
     </row>
     <row r="541" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E541" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="542" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E542" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="543" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E543" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="544" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E544" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="545" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E545" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="546" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E546" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="547" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E547" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="548" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E548" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
     </row>
     <row r="549" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E549" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="550" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E550" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
     </row>
     <row r="551" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E551" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
     </row>
     <row r="552" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E552" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="553" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E553" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="554" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E554" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="555" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E555" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="556" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E556" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="557" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E557" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="558" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E558" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="559" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E559" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
     </row>
     <row r="560" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E560" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="561" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E561" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="562" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E562" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="563" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E563" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
     <row r="564" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E564" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="565" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E565" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
     </row>
     <row r="566" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E566" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="567" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E567" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="568" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E568" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="569" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E569" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="570" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E570" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="571" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E571" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="572" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E572" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="573" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E573" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="574" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E574" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
     </row>
     <row r="575" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E575" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
     </row>
     <row r="576" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E576" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="577" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E577" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="578" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E578" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="579" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E579" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
     </row>
     <row r="580" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E580" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
     </row>
     <row r="581" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E581" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
     </row>
     <row r="582" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E582" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="583" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E583" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
     </row>
     <row r="584" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E584" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="585" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E585" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
     <row r="586" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6062,142 +6065,142 @@
     </row>
     <row r="587" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E587" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
     </row>
     <row r="588" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E588" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
     </row>
     <row r="589" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E589" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
     </row>
     <row r="590" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E590" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="591" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E591" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="592" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E592" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
     </row>
     <row r="593" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E593" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="594" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E594" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
     </row>
     <row r="595" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E595" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="596" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E596" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="597" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E597" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
     <row r="598" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E598" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
     </row>
     <row r="599" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E599" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="600" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E600" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="601" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E601" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="602" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E602" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="603" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E603" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
     </row>
     <row r="604" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E604" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
     </row>
     <row r="605" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E605" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="606" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E606" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="607" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E607" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
     <row r="608" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E608" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
     </row>
     <row r="609" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E609" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
     </row>
     <row r="610" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E610" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
     <row r="611" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E611" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="612" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E612" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
     </row>
     <row r="613" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E613" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
     <row r="614" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E614" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
     </row>
     <row r="615" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6212,137 +6215,142 @@
     </row>
     <row r="617" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E617" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
     </row>
     <row r="618" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E618" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
     </row>
     <row r="619" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E619" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
     </row>
     <row r="620" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E620" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
     </row>
     <row r="621" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E621" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
     </row>
     <row r="622" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E622" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="623" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E623" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
     </row>
     <row r="624" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E624" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
     </row>
     <row r="625" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E625" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="626" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E626" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="627" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E627" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
     </row>
     <row r="628" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E628" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
     </row>
     <row r="629" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E629" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
     </row>
     <row r="630" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E630" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
     </row>
     <row r="631" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E631" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
     </row>
     <row r="632" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E632" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
     </row>
     <row r="633" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E633" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
     </row>
     <row r="634" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E634" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
     </row>
     <row r="635" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E635" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
     </row>
     <row r="636" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E636" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
     </row>
     <row r="637" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E637" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
     </row>
     <row r="638" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E638" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
     </row>
     <row r="639" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E639" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
     </row>
     <row r="640" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E640" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
     </row>
     <row r="641" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E641" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
     </row>
     <row r="642" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E642" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
     </row>
     <row r="643" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E643" t="s">
-        <v>734</v>
+        <v>732</v>
+      </c>
+    </row>
+    <row r="644" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E644" t="s">
+        <v>735</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made some minor adjustments to the normalizations or words and more clean up work in the excel files
</commit_message>
<xml_diff>
--- a/1.Webscraper/Index.xlsx
+++ b/1.Webscraper/Index.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikol\Noty-Database\1.Webscraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94478FF-6A1F-4726-B780-8AE1DE8217CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACE642D-0900-4103-B3FF-BC9340D5C3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="736">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="926">
   <si>
     <t>Categories/Occasions</t>
   </si>
@@ -1170,9 +1170,6 @@
     <t>Александр Горянин</t>
   </si>
   <si>
-    <t>Джерела 277</t>
-  </si>
-  <si>
     <t>Е. Н. Пушков</t>
   </si>
   <si>
@@ -2248,6 +2245,579 @@
   </si>
   <si>
     <t>Razele cerului</t>
+  </si>
+  <si>
+    <t>L.M. Bauman</t>
+  </si>
+  <si>
+    <t>Марина Шрейнер</t>
+  </si>
+  <si>
+    <t>Л. Межохина</t>
+  </si>
+  <si>
+    <t>Ш. Гуно</t>
+  </si>
+  <si>
+    <t>Н. Давыденко</t>
+  </si>
+  <si>
+    <t>В. Перебиковский</t>
+  </si>
+  <si>
+    <t>А. Бабачук</t>
+  </si>
+  <si>
+    <t>Т. Спесивцева</t>
+  </si>
+  <si>
+    <t>F. Haydn</t>
+  </si>
+  <si>
+    <t>Т. Феттке</t>
+  </si>
+  <si>
+    <t>Rolf Løvland</t>
+  </si>
+  <si>
+    <t>П. Майборода</t>
+  </si>
+  <si>
+    <t>Оля Цуманчук</t>
+  </si>
+  <si>
+    <t>Веніамин Назарук</t>
+  </si>
+  <si>
+    <t>В. Яцюк</t>
+  </si>
+  <si>
+    <t>Гапонюк Андрей</t>
+  </si>
+  <si>
+    <t>Сергей Воробьёв</t>
+  </si>
+  <si>
+    <t>Песни юности</t>
+  </si>
+  <si>
+    <t>Євангельска Пісня</t>
+  </si>
+  <si>
+    <t>Ph. Bliss</t>
+  </si>
+  <si>
+    <t>Lee Mendelson</t>
+  </si>
+  <si>
+    <t>Vince Guaraldi</t>
+  </si>
+  <si>
+    <t>William J. Kirkpatrick</t>
+  </si>
+  <si>
+    <t>И Никита</t>
+  </si>
+  <si>
+    <t>M. Ghidora</t>
+  </si>
+  <si>
+    <t>V. Perebikovsky</t>
+  </si>
+  <si>
+    <t>I. Nichita</t>
+  </si>
+  <si>
+    <t>Placide Cappeau</t>
+  </si>
+  <si>
+    <t>Д. Ясько</t>
+  </si>
+  <si>
+    <t>Adolphe Adam</t>
+  </si>
+  <si>
+    <t>И. К. Гука</t>
+  </si>
+  <si>
+    <t>Caracciolo</t>
+  </si>
+  <si>
+    <t>M. Bass</t>
+  </si>
+  <si>
+    <t>A. Ryzhov D. Kort</t>
+  </si>
+  <si>
+    <t>P. Tsuman</t>
+  </si>
+  <si>
+    <t>T. Rusavuk</t>
+  </si>
+  <si>
+    <t>Anna W. Waterman</t>
+  </si>
+  <si>
+    <t>A.W. Waterman</t>
+  </si>
+  <si>
+    <t>M. Ledner</t>
+  </si>
+  <si>
+    <t>Arr. Edm. Fust</t>
+  </si>
+  <si>
+    <t>Т. С.</t>
+  </si>
+  <si>
+    <t>С. Бичковский</t>
+  </si>
+  <si>
+    <t>Парафейник</t>
+  </si>
+  <si>
+    <t>Тетяна Тарасюк</t>
+  </si>
+  <si>
+    <t>А. Гапонюк</t>
+  </si>
+  <si>
+    <t>Г. Везикова</t>
+  </si>
+  <si>
+    <t>И. Шевченко</t>
+  </si>
+  <si>
+    <t>А Краснокутский</t>
+  </si>
+  <si>
+    <t>Д. Мартынс</t>
+  </si>
+  <si>
+    <t>Л Симонова</t>
+  </si>
+  <si>
+    <t>Д Махмуд-Оглы</t>
+  </si>
+  <si>
+    <t>М. Гурлова</t>
+  </si>
+  <si>
+    <t>Л. Камалова</t>
+  </si>
+  <si>
+    <t>Т. Белозуб (Потаенко)</t>
+  </si>
+  <si>
+    <t>П Чесноков</t>
+  </si>
+  <si>
+    <t>С Воробьёв</t>
+  </si>
+  <si>
+    <t>Алена Долинина</t>
+  </si>
+  <si>
+    <t>J. Rutter</t>
+  </si>
+  <si>
+    <t>П.Я. Дацко</t>
+  </si>
+  <si>
+    <t>G. Davis</t>
+  </si>
+  <si>
+    <t>П. Дацко</t>
+  </si>
+  <si>
+    <t>Давис</t>
+  </si>
+  <si>
+    <t>Д. А. Ясько</t>
+  </si>
+  <si>
+    <t>Н. и Г.И. Адам</t>
+  </si>
+  <si>
+    <t>H. A. Lewis</t>
+  </si>
+  <si>
+    <t>И. Никита</t>
+  </si>
+  <si>
+    <t>И.С. Проханов</t>
+  </si>
+  <si>
+    <t>В.А. Агарков</t>
+  </si>
+  <si>
+    <t>Hedwig von Redern</t>
+  </si>
+  <si>
+    <t>Eugen Hecht</t>
+  </si>
+  <si>
+    <t>Л. Д. Нейкурс</t>
+  </si>
+  <si>
+    <t>Я. Крючковская</t>
+  </si>
+  <si>
+    <t>Группа Пилигрим</t>
+  </si>
+  <si>
+    <t>Л. Дарморост</t>
+  </si>
+  <si>
+    <t>Л. Халкиди</t>
+  </si>
+  <si>
+    <t>В. Юров</t>
+  </si>
+  <si>
+    <t>М. Джемикуловой</t>
+  </si>
+  <si>
+    <t>Р. Ахметшин</t>
+  </si>
+  <si>
+    <t>Л. Тимченко</t>
+  </si>
+  <si>
+    <t>Д Воробьёв</t>
+  </si>
+  <si>
+    <t>Л. Хархардина</t>
+  </si>
+  <si>
+    <t>J. Hoff</t>
+  </si>
+  <si>
+    <t>А. Чепуренко</t>
+  </si>
+  <si>
+    <t>Н. Драгня</t>
+  </si>
+  <si>
+    <t>Т. Потаенко</t>
+  </si>
+  <si>
+    <t>О. Данилова</t>
+  </si>
+  <si>
+    <t>П. Шабан</t>
+  </si>
+  <si>
+    <t>А. Зарецкий</t>
+  </si>
+  <si>
+    <t>обр. В. Гусаковой</t>
+  </si>
+  <si>
+    <t>Р Фот</t>
+  </si>
+  <si>
+    <t>Грибович</t>
+  </si>
+  <si>
+    <t>Переклад Л Одарчук</t>
+  </si>
+  <si>
+    <t>Т Альбинони</t>
+  </si>
+  <si>
+    <t>Н. Шибких</t>
+  </si>
+  <si>
+    <t>А. Денисова</t>
+  </si>
+  <si>
+    <t>Е. Разумовская</t>
+  </si>
+  <si>
+    <t>Е. Андрюхина</t>
+  </si>
+  <si>
+    <t>Л. Татаренко</t>
+  </si>
+  <si>
+    <t>М. Мельничук</t>
+  </si>
+  <si>
+    <t>Т. Квартальнова</t>
+  </si>
+  <si>
+    <t>Д. Балдин</t>
+  </si>
+  <si>
+    <t>Павел Кирнев</t>
+  </si>
+  <si>
+    <t>И. Крышко</t>
+  </si>
+  <si>
+    <t>Гоар Чайка</t>
+  </si>
+  <si>
+    <t>В. Стрелков</t>
+  </si>
+  <si>
+    <t>А. Гинтер</t>
+  </si>
+  <si>
+    <t>П. Цуман</t>
+  </si>
+  <si>
+    <t>П. Бальжик</t>
+  </si>
+  <si>
+    <t>О. Володина</t>
+  </si>
+  <si>
+    <t>Л. Е. К.</t>
+  </si>
+  <si>
+    <t>А. Димитров</t>
+  </si>
+  <si>
+    <t>Н.П. Ирецкая</t>
+  </si>
+  <si>
+    <t>А.С. Сычёв</t>
+  </si>
+  <si>
+    <t>Р. Е. П.</t>
+  </si>
+  <si>
+    <t>А. Чипилка</t>
+  </si>
+  <si>
+    <t>Гендель</t>
+  </si>
+  <si>
+    <t>П.М. Прудников</t>
+  </si>
+  <si>
+    <t>В.Ф. Миллер</t>
+  </si>
+  <si>
+    <t>Д. Литовченко</t>
+  </si>
+  <si>
+    <t>Л.М.</t>
+  </si>
+  <si>
+    <t>Л.К.</t>
+  </si>
+  <si>
+    <t>Песни Анны</t>
+  </si>
+  <si>
+    <t>И. Белоцкая</t>
+  </si>
+  <si>
+    <t>Р. Голкина</t>
+  </si>
+  <si>
+    <t>Л. Петько</t>
+  </si>
+  <si>
+    <t>Л. Гаврилюк (русский текст)</t>
+  </si>
+  <si>
+    <t>А. Лукашин</t>
+  </si>
+  <si>
+    <t>М. Халеева</t>
+  </si>
+  <si>
+    <t>Л. Алтухова</t>
+  </si>
+  <si>
+    <t>M. Cox</t>
+  </si>
+  <si>
+    <t>Л. Семлек</t>
+  </si>
+  <si>
+    <t>П. Чайковский</t>
+  </si>
+  <si>
+    <t>Д. Простомолотов</t>
+  </si>
+  <si>
+    <t>Ан. Г.</t>
+  </si>
+  <si>
+    <t>Ипполитов-Иванов</t>
+  </si>
+  <si>
+    <t>Г. А. К.</t>
+  </si>
+  <si>
+    <t>Т. Фетке</t>
+  </si>
+  <si>
+    <t>Анна Грибанова</t>
+  </si>
+  <si>
+    <t>Павел Сидько</t>
+  </si>
+  <si>
+    <t>А. Крючков</t>
+  </si>
+  <si>
+    <t>М. Патрашко</t>
+  </si>
+  <si>
+    <t>Петро Олійник</t>
+  </si>
+  <si>
+    <t>В. Сыч</t>
+  </si>
+  <si>
+    <t>В. Скумбин</t>
+  </si>
+  <si>
+    <t>А. Гантовник</t>
+  </si>
+  <si>
+    <t>Испанская мелодия</t>
+  </si>
+  <si>
+    <t>Цуман П.</t>
+  </si>
+  <si>
+    <t>Т Спесивцева</t>
+  </si>
+  <si>
+    <t>Т. Далина (обработка)</t>
+  </si>
+  <si>
+    <t>Л. Пашко (Украинские слова)</t>
+  </si>
+  <si>
+    <t>В. В. Перебиковский</t>
+  </si>
+  <si>
+    <t>В.Н. Степанов</t>
+  </si>
+  <si>
+    <t>Е. Бондарева</t>
+  </si>
+  <si>
+    <t>Чесноков (требуется доработка нот)</t>
+  </si>
+  <si>
+    <t>ЕП</t>
+  </si>
+  <si>
+    <t>ДН</t>
+  </si>
+  <si>
+    <t>В. Переверзев</t>
+  </si>
+  <si>
+    <t>В. Згодько</t>
+  </si>
+  <si>
+    <t>Cindy Berry</t>
+  </si>
+  <si>
+    <t>А. Кадацкая</t>
+  </si>
+  <si>
+    <t>А.П. Яворивский</t>
+  </si>
+  <si>
+    <t>Маген Станислав</t>
+  </si>
+  <si>
+    <t>John E. Walvoord</t>
+  </si>
+  <si>
+    <t>Don Wyrtzen</t>
+  </si>
+  <si>
+    <t>А. Гордеев</t>
+  </si>
+  <si>
+    <t>Л.В. Бетховен (Хор и фортепиано)</t>
+  </si>
+  <si>
+    <t>Елена Дюкова</t>
+  </si>
+  <si>
+    <t>В.И. Павлов</t>
+  </si>
+  <si>
+    <t>Маршнер</t>
+  </si>
+  <si>
+    <t>С.А. Бацук</t>
+  </si>
+  <si>
+    <t>Гр. Кендрик</t>
+  </si>
+  <si>
+    <t>J. H. Tenney</t>
+  </si>
+  <si>
+    <t>Денис Пацюк</t>
+  </si>
+  <si>
+    <t>Ph.P. Bliss</t>
+  </si>
+  <si>
+    <t>Г. Конради</t>
+  </si>
+  <si>
+    <t>J. Macy</t>
+  </si>
+  <si>
+    <t>Народная мел.</t>
+  </si>
+  <si>
+    <t>Dan and Heidi Goeller</t>
+  </si>
+  <si>
+    <t>Е. Кашина</t>
+  </si>
+  <si>
+    <t>С. Шинкарёва</t>
+  </si>
+  <si>
+    <t>А. Каргопольцев</t>
+  </si>
+  <si>
+    <t>В. Петреченко</t>
+  </si>
+  <si>
+    <t>Еврейская мелодия</t>
+  </si>
+  <si>
+    <t>В. Мысин</t>
+  </si>
+  <si>
+    <t>Гурт Ковчег</t>
+  </si>
+  <si>
+    <t>Н. Николенко</t>
+  </si>
+  <si>
+    <t>Л. Клочкова</t>
+  </si>
+  <si>
+    <t>Скрипичный</t>
+  </si>
+  <si>
+    <t>М. Кривошеев</t>
+  </si>
+  <si>
+    <t>K. Hipke (Chamber)</t>
+  </si>
+  <si>
+    <t>Ю. Аксенова</t>
   </si>
 </sst>
 </file>
@@ -2591,10 +3161,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G644"/>
+  <dimension ref="A1:G864"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C640" workbookViewId="0">
-      <selection activeCell="E648" sqref="E648"/>
+    <sheetView tabSelected="1" topLeftCell="B854" workbookViewId="0">
+      <selection activeCell="G858" sqref="G858"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2697,7 +3267,7 @@
         <v>132</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2720,7 +3290,7 @@
         <v>133</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2829,7 +3399,7 @@
         <v>114</v>
       </c>
       <c r="E10" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="F10" t="s">
         <v>145</v>
@@ -2881,7 +3451,7 @@
         <v>149</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2921,7 +3491,7 @@
         <v>196</v>
       </c>
       <c r="F14" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2941,7 +3511,7 @@
         <v>197</v>
       </c>
       <c r="F15" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2961,7 +3531,7 @@
         <v>178</v>
       </c>
       <c r="F16" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3001,7 +3571,7 @@
         <v>198</v>
       </c>
       <c r="F18" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3015,7 +3585,7 @@
         <v>62</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E19" t="s">
         <v>199</v>
@@ -3040,6 +3610,9 @@
       <c r="E20" t="s">
         <v>200</v>
       </c>
+      <c r="F20" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
@@ -3052,10 +3625,13 @@
         <v>64</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="E21" t="s">
         <v>201</v>
+      </c>
+      <c r="F21" t="s">
+        <v>753</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3069,7 +3645,7 @@
         <v>65</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="E22" t="s">
         <v>202</v>
@@ -3085,7 +3661,9 @@
       <c r="C23" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="2"/>
+      <c r="D23" s="2" t="s">
+        <v>880</v>
+      </c>
       <c r="E23" t="s">
         <v>203</v>
       </c>
@@ -3098,7 +3676,9 @@
       <c r="C24" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="2"/>
+      <c r="D24" s="2" t="s">
+        <v>917</v>
+      </c>
       <c r="E24" t="s">
         <v>204</v>
       </c>
@@ -3372,7 +3952,7 @@
     </row>
     <row r="48" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C48" s="2" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="E48" t="s">
         <v>220</v>
@@ -4270,192 +4850,192 @@
     </row>
     <row r="227" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E227" t="s">
-        <v>376</v>
+        <v>922</v>
       </c>
     </row>
     <row r="228" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E228" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="229" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E229" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="230" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E230" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="231" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E231" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="232" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E232" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="233" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E233" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="234" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E234" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="235" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E235" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="236" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E236" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="237" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E237" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="238" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E238" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="239" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E239" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="240" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E240" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="241" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E241" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="242" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E242" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="243" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E243" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="244" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E244" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="245" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E245" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="246" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E246" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="247" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E247" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="248" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E248" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="249" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E249" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="250" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E250" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="251" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E251" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="252" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E252" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="253" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E253" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="254" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E254" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="255" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E255" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="256" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E256" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="257" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E257" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="258" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E258" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="259" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E259" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="260" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E260" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="261" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E261" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="262" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E262" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="263" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E263" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="264" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E264" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="265" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4465,17 +5045,17 @@
     </row>
     <row r="266" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E266" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="267" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E267" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="268" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E268" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="269" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4485,12 +5065,12 @@
     </row>
     <row r="270" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E270" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="271" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E271" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="272" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4500,132 +5080,132 @@
     </row>
     <row r="273" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E273" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="274" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E274" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="275" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E275" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="276" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E276" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="277" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E277" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="278" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E278" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="279" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E279" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="280" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E280" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="281" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E281" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="282" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E282" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="283" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E283" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="284" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E284" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="285" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E285" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="286" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E286" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="287" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E287" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="288" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E288" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="289" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E289" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="290" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E290" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="291" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E291" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="292" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E292" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="293" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E293" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="294" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E294" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="295" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E295" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="296" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E296" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="297" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E297" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="298" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E298" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="299" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4635,77 +5215,77 @@
     </row>
     <row r="300" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E300" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="301" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E301" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="302" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E302" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="303" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E303" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="304" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E304" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="305" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E305" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="306" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E306" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="307" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E307" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="308" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E308" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="309" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E309" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="310" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E310" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="311" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E311" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="312" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E312" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="313" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E313" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="314" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E314" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="315" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4720,42 +5300,42 @@
     </row>
     <row r="317" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E317" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="318" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E318" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="319" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E319" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="320" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E320" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="321" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E321" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="322" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E322" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="323" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E323" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="324" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E324" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="325" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4765,522 +5345,522 @@
     </row>
     <row r="326" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E326" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="327" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E327" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="328" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E328" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="329" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E329" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="330" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E330" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="331" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E331" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="332" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E332" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="333" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E333" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="334" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E334" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="335" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E335" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="336" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E336" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="337" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E337" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="338" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E338" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="339" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E339" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="340" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E340" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="341" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E341" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="342" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E342" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="343" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E343" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="344" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E344" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="345" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E345" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="346" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E346" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="347" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E347" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="348" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E348" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="349" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E349" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="350" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E350" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="351" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E351" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="352" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E352" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="353" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E353" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="354" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E354" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="355" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E355" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="356" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E356" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="357" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E357" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="358" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E358" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="359" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E359" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="360" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E360" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="361" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E361" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="362" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E362" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="363" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E363" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="364" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E364" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="365" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E365" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="366" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E366" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="367" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E367" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="368" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E368" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="369" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E369" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="370" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E370" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="371" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E371" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="372" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E372" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="373" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E373" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="374" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E374" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="375" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E375" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="376" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E376" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="377" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E377" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="378" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E378" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="379" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E379" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="380" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E380" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="381" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E381" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="382" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E382" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="383" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E383" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="384" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E384" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="385" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E385" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="386" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E386" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="387" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E387" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="388" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E388" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="389" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E389" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="390" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E390" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="391" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E391" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="392" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E392" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="393" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E393" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="394" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E394" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="395" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E395" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="396" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E396" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="397" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E397" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="398" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E398" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="399" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E399" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="400" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E400" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="401" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E401" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="402" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E402" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="403" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E403" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="404" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E404" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="405" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E405" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="406" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E406" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="407" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E407" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="408" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E408" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="409" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E409" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="410" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E410" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="411" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E411" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="412" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E412" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="413" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E413" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="414" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E414" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="415" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E415" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="416" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E416" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="417" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E417" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="418" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E418" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="419" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E419" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="420" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E420" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="421" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E421" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="422" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E422" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="423" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E423" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="424" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E424" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="425" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E425" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="426" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E426" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="427" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E427" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="428" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E428" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="429" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E429" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="430" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5290,92 +5870,92 @@
     </row>
     <row r="431" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E431" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="432" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E432" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="433" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E433" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="434" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E434" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="435" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E435" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="436" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E436" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="437" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E437" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="438" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E438" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="439" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E439" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="440" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E440" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="441" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E441" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="442" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E442" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="443" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E443" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="444" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E444" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="445" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E445" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="446" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E446" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="447" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E447" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="448" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E448" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="449" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5385,12 +5965,12 @@
     </row>
     <row r="450" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E450" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="451" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E451" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="452" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5405,12 +5985,12 @@
     </row>
     <row r="454" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E454" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="455" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E455" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="456" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5420,87 +6000,87 @@
     </row>
     <row r="457" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E457" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="458" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E458" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="459" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E459" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="460" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E460" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="461" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E461" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="462" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E462" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="463" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E463" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="464" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E464" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="465" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E465" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="466" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E466" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="467" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E467" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="468" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E468" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="469" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E469" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="470" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E470" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="471" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E471" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="472" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E472" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="473" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E473" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="474" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5510,102 +6090,102 @@
     </row>
     <row r="475" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E475" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="476" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E476" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="477" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E477" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="478" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E478" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="479" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E479" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="480" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E480" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="481" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E481" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="482" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E482" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="483" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E483" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="484" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E484" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="485" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E485" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="486" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E486" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="487" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E487" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="488" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E488" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="489" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E489" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="490" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E490" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="491" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E491" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="492" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E492" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="493" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E493" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="494" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E494" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="495" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5615,87 +6195,92 @@
     </row>
     <row r="496" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E496" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="497" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E497" t="s">
-        <v>628</v>
+        <v>627</v>
+      </c>
+    </row>
+    <row r="498" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E498" t="s">
+        <v>921</v>
       </c>
     </row>
     <row r="499" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E499" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="500" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E500" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="501" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E501" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="502" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E502" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="503" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E503" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="504" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E504" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="505" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E505" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="506" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E506" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="507" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E507" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="508" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E508" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="509" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E509" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="510" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E510" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="511" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E511" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="512" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E512" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="513" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E513" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="514" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5705,27 +6290,27 @@
     </row>
     <row r="515" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E515" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="516" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E516" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="517" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E517" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="518" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E518" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="519" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E519" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="520" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5735,327 +6320,327 @@
     </row>
     <row r="521" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E521" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="522" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E522" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="523" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E523" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="524" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E524" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="525" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E525" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="526" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E526" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="527" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E527" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="528" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E528" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="529" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E529" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="530" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E530" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="531" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E531" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="532" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E532" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="533" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E533" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="534" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E534" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="535" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E535" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="536" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E536" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="537" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E537" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="538" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E538" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="539" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E539" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="540" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E540" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="541" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E541" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="542" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E542" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="543" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E543" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="544" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E544" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="545" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E545" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="546" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E546" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="547" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E547" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="548" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E548" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="549" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E549" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="550" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E550" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="551" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E551" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="552" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E552" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="553" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E553" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="554" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E554" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="555" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E555" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="556" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E556" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="557" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E557" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="558" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E558" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="559" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E559" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="560" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E560" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="561" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E561" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="562" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E562" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="563" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E563" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="564" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E564" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="565" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E565" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="566" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E566" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="567" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E567" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="568" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E568" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="569" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E569" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="570" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E570" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="571" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E571" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="572" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E572" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="573" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E573" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="574" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E574" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="575" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E575" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="576" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E576" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="577" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E577" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="578" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E578" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="579" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E579" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="580" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E580" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="581" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E581" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="582" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E582" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="583" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E583" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="584" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E584" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="585" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E585" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="586" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6065,142 +6650,142 @@
     </row>
     <row r="587" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E587" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="588" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E588" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="589" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E589" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="590" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E590" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="591" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E591" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="592" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E592" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="593" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E593" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="594" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E594" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="595" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E595" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="596" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E596" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="597" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E597" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="598" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E598" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="599" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E599" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="600" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E600" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="601" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E601" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="602" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E602" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="603" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E603" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="604" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E604" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="605" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E605" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="606" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E606" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="607" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E607" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="608" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E608" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="609" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E609" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="610" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E610" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="611" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E611" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="612" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E612" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="613" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E613" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="614" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E614" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="615" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6215,142 +6800,1242 @@
     </row>
     <row r="617" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E617" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="618" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E618" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="619" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E619" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="620" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E620" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="621" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E621" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="622" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E622" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="623" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E623" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="624" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E624" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="625" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E625" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="626" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E626" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="627" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E627" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="628" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E628" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="629" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E629" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="630" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E630" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="631" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E631" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="632" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E632" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="633" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E633" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="634" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E634" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="635" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E635" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="636" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E636" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="637" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E637" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="638" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E638" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="639" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E639" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="640" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E640" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="641" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E641" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="642" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E642" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="643" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E643" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="644" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E644" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="645" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E645" t="s">
         <v>735</v>
+      </c>
+    </row>
+    <row r="646" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E646" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="647" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E647" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="648" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E648" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="649" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E649" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="650" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E650" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="651" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E651" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="652" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E652" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="653" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E653" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="654" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E654" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="655" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E655" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="656" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E656" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="657" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E657" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="658" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E658" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="659" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E659" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="660" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E660" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="661" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E661" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="662" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E662" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="663" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E663" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="664" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E664" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="665" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E665" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="666" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E666" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="667" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E667" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="668" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E668" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="669" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E669" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="670" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E670" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="671" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E671" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="672" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E672" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="673" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E673" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="674" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E674" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="675" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E675" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="676" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E676" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="677" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E677" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="678" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E678" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="679" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E679" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="680" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E680" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="681" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E681" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="682" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E682" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="683" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E683" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="684" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E684" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="685" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E685" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="686" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E686" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="687" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E687" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="688" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E688" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="689" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E689" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="690" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E690" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="691" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E691" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="692" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E692" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="693" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E693" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="694" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E694" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="695" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E695" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="696" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E696" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="697" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E697" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="698" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E698" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="699" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E699" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="700" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E700" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="701" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E701" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="702" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E702" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="703" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E703" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="704" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E704" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="705" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E705" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="706" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E706" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="707" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E707" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="708" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E708" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="709" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E709" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="710" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E710" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="711" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E711" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="712" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E712" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="713" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E713" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="714" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E714" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="715" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E715" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="716" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E716" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="717" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E717" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="718" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E718" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="719" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E719" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="720" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E720" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="721" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E721" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="722" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E722" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="723" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E723" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="724" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E724" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="725" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E725" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="726" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E726" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="727" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E727" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="728" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E728" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="729" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E729" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="730" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E730" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="731" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E731" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="732" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E732" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="733" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E733" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="734" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E734" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="735" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E735" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="736" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E736" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="737" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E737" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="738" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E738" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="739" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E739" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="740" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E740" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="741" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E741" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="742" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E742" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="743" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E743" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="744" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E744" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="745" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E745" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="746" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E746" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="747" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E747" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="748" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E748" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="749" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E749" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="750" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E750" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="751" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E751" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="752" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E752" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="753" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E753" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="754" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E754" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="755" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E755" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="756" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E756" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="757" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E757" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="758" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E758" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="759" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E759" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="760" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E760" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="761" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E761" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="762" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E762" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="763" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E763" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="764" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E764" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="765" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E765" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="766" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E766" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="767" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E767" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="768" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E768" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="769" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E769" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="770" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E770" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="771" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E771" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="772" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E772" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="773" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E773" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="774" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E774" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="775" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E775" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="776" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E776" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="777" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E777" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="778" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E778" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="779" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E779" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="780" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E780" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="781" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E781" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="782" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E782" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="783" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E783" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="784" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E784" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="785" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E785" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="786" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E786" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="787" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E787" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="788" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E788" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="789" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E789" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="790" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E790" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="791" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E791" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="792" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E792" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="793" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E793" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="794" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E794" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="795" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E795" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="796" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E796" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="797" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E797" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="798" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E798" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="799" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E799" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="800" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E800" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="801" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E801" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="802" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E802" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="803" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E803" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="804" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E804" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="805" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E805" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="806" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E806" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="807" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E807" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="808" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E808" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="809" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E809" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="810" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E810" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="811" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E811" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="812" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E812" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="813" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E813" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="814" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E814" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="815" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E815" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="816" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E816" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="817" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E817" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="818" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E818" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="819" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E819" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="820" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E820" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="821" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E821" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="822" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E822" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="823" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E823" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="824" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E824" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="825" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E825" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="826" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E826" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="827" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E827" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="828" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E828" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="829" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E829" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="830" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E830" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="831" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E831" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="832" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E832" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="833" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E833" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="834" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E834" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="835" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E835" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="836" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E836" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="837" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E837" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="838" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E838" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="839" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E839" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="840" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E840" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="841" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E841" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="842" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E842" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="843" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E843" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="844" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E844" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="845" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E845" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="846" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E846" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="847" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E847" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="848" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E848" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="849" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E849" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="850" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E850" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="851" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E851" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="852" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E852" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="853" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E853" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="854" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E854" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="855" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E855" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="856" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E856" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="857" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E857" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="858" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E858" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="859" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E859" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="860" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E860" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="861" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E861" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="862" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E862" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="863" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E863" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="864" spans="5:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E864" t="s">
+        <v>920</v>
       </c>
     </row>
   </sheetData>

</xml_diff>